<commit_message>
Added timestamp support. Refactored code.
</commit_message>
<xml_diff>
--- a/PandasDFChallenge_(7.10.2024)_github/data/dataTables.xlsx
+++ b/PandasDFChallenge_(7.10.2024)_github/data/dataTables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talba\Documents\Coding_Projects\Python\My Own\PandasDFChallenge_(30.9.2024) - improved\PandasDFChallenge_(30.9.2024)\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talba\Documents\Coding_Projects\Python\My Own\PandasDFChallenge_(30.9.2024)_with_git\PandasDFChallenge_(30.9.2024)\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C811B7-386E-425E-B8AF-EED49EDDB661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976B97CB-5F7B-4777-AB98-79C7DE45B2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{B5FC0206-FA51-4BD3-AC86-D580FCB947D7}"/>
   </bookViews>
@@ -138,12 +138,48 @@
       <charset val="177"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -158,8 +194,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF4CD99-BC8A-4EC7-9E9F-5D1BCF8D8DC3}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C25" sqref="C25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -503,7 +545,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>123</v>
       </c>
       <c r="B2">
@@ -520,11 +562,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>679</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>178</v>
@@ -537,11 +579,11 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>453</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>63.2</v>
@@ -554,11 +596,11 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>452</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>34</v>
@@ -571,11 +613,11 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>123</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>50</v>
@@ -588,11 +630,11 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>123</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>49</v>
@@ -605,11 +647,11 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>452</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>39</v>
@@ -622,11 +664,11 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>123</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>50</v>
@@ -639,11 +681,11 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>679</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>161.4</v>
@@ -656,11 +698,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>679</v>
       </c>
       <c r="B11">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>173.7</v>
@@ -673,11 +715,11 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>123</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>56</v>
@@ -690,11 +732,11 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>453</v>
       </c>
       <c r="B13">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>72</v>
@@ -707,11 +749,11 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>453</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>70</v>
@@ -724,11 +766,11 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>452</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>67</v>
@@ -741,11 +783,11 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>123</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>63.2</v>
@@ -758,11 +800,11 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="A17" s="5">
         <v>998</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C17">
         <v>110</v>
@@ -775,11 +817,11 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="A18" s="3">
         <v>453</v>
       </c>
       <c r="B18">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>67.3</v>
@@ -792,11 +834,11 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="A19" s="5">
         <v>998</v>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C19">
         <v>87.4</v>
@@ -809,11 +851,11 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>123</v>
       </c>
       <c r="B20">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C20">
         <v>67</v>
@@ -826,11 +868,11 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="A21" s="5">
         <v>998</v>
       </c>
       <c r="B21">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>50</v>
@@ -843,11 +885,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="A22" s="5">
         <v>998</v>
       </c>
       <c r="B22">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>50</v>
@@ -860,11 +902,11 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>66666</v>
+      <c r="A23" s="6">
+        <v>666</v>
       </c>
       <c r="B23">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C23">
         <v>50</v>
@@ -874,6 +916,40 @@
       </c>
       <c r="E23">
         <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="5">
+        <v>343</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>63.2</v>
+      </c>
+      <c r="D24">
+        <v>71</v>
+      </c>
+      <c r="E24">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="5">
+        <v>343</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>50</v>
+      </c>
+      <c r="D25">
+        <v>77</v>
+      </c>
+      <c r="E25">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -887,7 +963,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>